<commit_message>
Exportar a XML con Schema
</commit_message>
<xml_diff>
--- a/sinnada.xlsx
+++ b/sinnada.xlsx
@@ -14,18 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>none</t>
   </si>
   <si>
-    <t>datito2</t>
-  </si>
-  <si>
-    <t>datoto3</t>
-  </si>
-  <si>
-    <t>datkoiaj2</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Edad</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
   </si>
 </sst>
 </file>
@@ -337,12 +340,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.143973214285714" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="10.001116071428571" style="0" customWidth="1"/>
-    <col min="2" max="2" width="10.858258928571429" style="0" customWidth="1"/>
-    <col min="3" max="3" width="12.858258928571429" style="0" customWidth="1"/>
+    <col min="1" max="2" width="9.143973214285714" style="0" customWidth="1"/>
+    <col min="3" max="3" width="9.715401785714286" style="0" customWidth="1"/>
+    <col min="4" max="4" width="9.143973214285714" style="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.0">
+    <row r="1" ht="15.0">
       <c r="A1" s="0" t="s">
         <v>1</v>
       </c>
@@ -352,6 +355,9 @@
       <c r="C1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Exportacion a XML avance 2
</commit_message>
<xml_diff>
--- a/sinnada.xlsx
+++ b/sinnada.xlsx
@@ -19,7 +19,7 @@
     <t>none</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>Nombre</t>
   </si>
   <si>
     <t>Edad</t>
@@ -28,7 +28,7 @@
     <t>Telefono</t>
   </si>
   <si>
-    <t>Ciudad</t>
+    <t>SaldoCuenta</t>
   </si>
 </sst>
 </file>
@@ -342,7 +342,7 @@
   <cols>
     <col min="1" max="2" width="9.143973214285714" style="0" customWidth="1"/>
     <col min="3" max="3" width="9.715401785714286" style="0" customWidth="1"/>
-    <col min="4" max="4" width="9.143973214285714" style="0" customWidth="1"/>
+    <col min="4" max="4" width="14.286830357142858" style="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.0">

</xml_diff>

<commit_message>
Cambios Estandarizacion Avance 3
</commit_message>
<xml_diff>
--- a/sinnada.xlsx
+++ b/sinnada.xlsx
@@ -22,13 +22,13 @@
     <t>Nombre</t>
   </si>
   <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>Cel</t>
+  </si>
+  <si>
     <t>Edad</t>
-  </si>
-  <si>
-    <t>Telefono</t>
-  </si>
-  <si>
-    <t>SaldoCuenta</t>
   </si>
 </sst>
 </file>
@@ -340,9 +340,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.143973214285714" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="9.143973214285714" style="0" customWidth="1"/>
-    <col min="3" max="3" width="9.715401785714286" style="0" customWidth="1"/>
-    <col min="4" max="4" width="14.286830357142858" style="0" customWidth="1"/>
+    <col min="1" max="1" width="9.143973214285714" style="0" customWidth="1"/>
+    <col min="2" max="2" width="9.286830357142858" style="0" customWidth="1"/>
+    <col min="3" max="4" width="9.143973214285714" style="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.0">

</xml_diff>